<commit_message>
fix: Update folder path in folder path.txt to reflect new directory structure
</commit_message>
<xml_diff>
--- a/check/Master Index.xlsx
+++ b/check/Master Index.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IDM252577\Desktop\Code\sortx\check\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\sortx\check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6C31C7-544A-44D0-89B6-0D575F2527A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4375FBCD-42D1-4396-A73F-902A04B8ACB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="936" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ASWXL.Storage" sheetId="5" state="veryHidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>ELECTRICAL</t>
   </si>
   <si>
-    <t>Needlist-1</t>
-  </si>
-  <si>
     <t>S.No.</t>
   </si>
   <si>
@@ -54,45 +51,15 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Doc. No.</t>
-  </si>
-  <si>
-    <t>Rev</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>Need List Name</t>
-  </si>
-  <si>
-    <t>NL Batch</t>
-  </si>
-  <si>
     <t>OVERALL SINGLE LINE DIAGRAM 380V MSB</t>
   </si>
   <si>
-    <t>00S4620-51-E-32-004_01</t>
-  </si>
-  <si>
-    <t>ABK-NEED LIST_05.xlsx</t>
-  </si>
-  <si>
     <t>Overall Single Line Diagram (380 Main SB)</t>
   </si>
   <si>
-    <t>00S4620-51-E-32-004_01r2</t>
-  </si>
-  <si>
     <t>EB-1801 6,6 KV SWB METERING AND PROTECTION</t>
   </si>
   <si>
-    <t>N-A18-EL-SLD-43-002</t>
-  </si>
-  <si>
     <t>H-0830 ELECTRICAL CABIN EQUIPMENT LAYOUT</t>
   </si>
   <si>
@@ -111,9 +78,6 @@
     <t>M-A26-EL-LYT-43-312</t>
   </si>
   <si>
-    <t>M-A27-EL-LYT-43-410</t>
-  </si>
-  <si>
     <t>ELECTRICAL EQUIPMENT LAYOUT AND CABLE ROUTE - MEZZANINE, UPPER AND HELI DECK</t>
   </si>
   <si>
@@ -132,67 +96,34 @@
     <t>Processed Date</t>
   </si>
   <si>
-    <t>Site</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>File count</t>
   </si>
   <si>
-    <t>ABK</t>
-  </si>
-  <si>
-    <t>Layout</t>
-  </si>
-  <si>
-    <t>SLD</t>
-  </si>
-  <si>
-    <t>T:\Project\aeT00989.00 Decarbonization Feasibility Study\06. Tebodin Design Information (No products)\6.01 General\Data Sorted\ELECTRICAL\ABK\SLD\00S4620-51-E-32-004_01</t>
-  </si>
-  <si>
-    <t>T:\Project\aeT00989.00 Decarbonization Feasibility Study\06. Tebodin Design Information (No products)\6.01 General\Data Sorted\ELECTRICAL\ABK\SLD\00S4620-51-E-32-004_01r2</t>
-  </si>
-  <si>
-    <t>T:\Project\aeT00989.00 Decarbonization Feasibility Study\06. Tebodin Design Information (No products)\6.01 General\Data Sorted\ELECTRICAL\ABK\Uncategorized\N-A18-EL-SLD-43-002</t>
-  </si>
-  <si>
-    <t>T:\Project\aeT00989.00 Decarbonization Feasibility Study\06. Tebodin Design Information (No products)\6.01 General\Data Sorted\ELECTRICAL\ABK\Layout\ABK0908-08-E-38-050_03-03</t>
-  </si>
-  <si>
-    <t>T:\Project\aeT00989.00 Decarbonization Feasibility Study\06. Tebodin Design Information (No products)\6.01 General\Data Sorted\ELECTRICAL\ABK\Layout\M-A26-EL-LYT-43-311</t>
-  </si>
-  <si>
-    <t>T:\Project\aeT00989.00 Decarbonization Feasibility Study\06. Tebodin Design Information (No products)\6.01 General\Data Sorted\ELECTRICAL\ABK\Layout\M-A26-EL-LYT-43-312</t>
-  </si>
-  <si>
-    <t>T:\Project\aeT00989.00 Decarbonization Feasibility Study\06. Tebodin Design Information (No products)\6.01 General\Data Sorted\ELECTRICAL\ABK\Layout\M-A27-EL-LYT-43-410</t>
-  </si>
-  <si>
-    <t>T:\Project\aeT00989.00 Decarbonization Feasibility Study\06. Tebodin Design Information (No products)\6.01 General\Data Sorted\ELECTRICAL\ABK\Layout\M-A27-EL-LYT-43-411</t>
-  </si>
-  <si>
-    <t>T:\Project\aeT00989.00 Decarbonization Feasibility Study\06. Tebodin Design Information (No products)\6.01 General\Data Sorted\ELECTRICAL\ABK\Layout\M-A28-EL-LYT-43-510</t>
-  </si>
-  <si>
-    <t>T:\Project\aeT00989.00 Decarbonization Feasibility Study\06. Tebodin Design Information (No products)\6.01 General\Data Sorted\ELECTRICAL\ABK\Layout\M-A28-EL-LYT-43-511</t>
-  </si>
-  <si>
-    <t>T:\Project\aeT00989.00 Decarbonization Feasibility Study\06. Tebodin Design Information (No products)\6.01 General\Data Sorted\ELECTRICAL\ABK\Layout\M-A29-EL-LYT-43-610</t>
-  </si>
-  <si>
     <t>File Path</t>
   </si>
   <si>
-    <t>ASWXL Storage Version 38.0.0.0</t>
-  </si>
-  <si>
-    <t>C:\Program Files (x86)\AspenTech\Aspen Simulation Workbook V12.0</t>
-  </si>
-  <si>
-    <t>UEsDBBQAAAAIAIldt1bRwGiWzhIAAF/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9tGlqcsyTpsK3I88eSwZ1iqbNXslqzTjh2V5JRMWQ4rkqWIip2Uy8W0gCYJC0AzDUBH/oz9P/bezd7HzB4ze8/svTt7fNiv82G/zUdvv8bVAEGKpAACE0MqQXjdr7t//fr164fXDbIwVCgUXrIf+A8/ly+wy2frRhPr+1hqzK1Xnn66Nbcuy4o+W3yCqaEQfW353twC/M4WS5ZqWhSv6dgyKVJni7vWgapIH+HTfXKI9bUFJEl3lqWFe+/XlhbuybVRaOfNcPVPCT08IOTwGsscrh5Jl6uGolkqMlljxtUqkkzlCFe8pMvVJsU1TLEuYeNyVdEVU0Gq8iWWp6oaMkxMN5CJKti8HiTnHPxvCMklopuUqCqmV6oU6XW8jXRUx/RytU6J1VyXWBPGtSqyTKKxxqV9VP+kKSMT36xuYBWbeB8dqPhpA+ucVPT6HtTyc1WLcz08kbC6aekS7wqw7bCuu/19u2qgI7yl6IdYZt3bYXXwvrKCN3jWQ+0Ay3JL5rerNUIlvGmp6h6uUWw0dvQ9Sy8RrQmQZBAZ4N7ECEZnGzWvV03A+UBF+mGJqNBrrJvG21VkHPMerHOEu0jHD3Wg5ZGRCyMF9jsyYivGyHBhJjxuTxBVgLkEAuQVgPbcCbP52Yad4g9lsOS74ZK73jgHGYe+FeaEsbRv4Q54xr/TmccfeeC+EWbeE5QBGN4JMzzy9YND4j/FlpkTGghg/Wq4csr0TwsI5hHWMVWkuQ2FJyB6+vnSs2cOY8WkTLNmi5ohEaoqB/5UvN3tTDy4exfdke68t/j+8m3M5uPz2We9oijr5vJSQiB2Dl4wDPFW/jzm6oZg8CaG4QKTYnJiFMZ94iJcIXEMLuPsMvpTZlE7KQywjx0h1cLVamEcqoVamQ6xiiYmoZpLQI5Capez7mIVUYpOL1YlYunmSKu+lt1yz57z6cE7c9kx+6Mj55q44cZvtjTulxSbv+I2P9rt7AcZT24RJG8yY0jomDOs42D7EMV0+kNkNEpExruUHCkypuOQUGGLwwgbWePiExC6weQ9zBq9NH4jYg6U3brejcpsqR868pOP730A/Zic5NoxBZfXoF+gG2fYKijxTXeF2sMagUXE6dbEp5pakRpYQ5fY3YZSqz2iSBseGppyoDl8XJjTMBBX2eX/fnxh9YMTTS0eOTo/szi3MFNkgiRsGa+vzVhm7dbiezMf3L8yuXpirBi8haIir814qGaKJqJ1bD5GGjaaSMJrMw3TbK7Mz7NmmxZV5gitzwOngc3FuRNDnimyJnVjRTNM3eiWu+taT3zW4+PjueNlzrm0sLA4/+n2li0jHwFbehHrJtWdvhm3NEWixCA185ZEtBXGd8vm8ss0KWmeXQa4ZorIZAb5wDLxJqHaBq4hZkvWZr6wmBdSUzADzXwBjS2wbbKZ3ItFkLzDVtSZlAPCt8GtlA1HMdZmTGphL/0TA5csyqaGuUUkpGInm9dr1yxxX+Bk/7SJnVQnvUEUCRc1Rd+RJIsyqTLN0NCJS1n6AZvCsgvSLxiEytwg15wAKJDKiqBtS2Lp9oD8XAN/YcFED2VFNV3e8MSwh5G8o6unIemsM2etrEuUl3LzTNbw2gyrTdFNj7N3HZ/vAiHUJzRo8MU74TY3sCFRpQlGKs6mg3rSDRBuYAUIMrEcJRkYhE/YA4GRrhQ+hrlunqYLgjsc6ULgXvQAx2J1vp0x4TnRRohnObi7sHr77azewitt9TJjgbjOpQuBOYkfslHCdI8cC0jYM7+KEROP7PoENaQagzWODJowUtnDB2oMbhMy0x3CB4Sy8Vun4A3FNo/6E8dTRTYbGRsmbgQr5qma8kzbV8xM4IDpztrMAJKyrmNqa2+KeruNWRvrulxiSQEgnvIOEEzFRKYV5YV4E2jno599l2RLMcwEPRDeBrghA/QpSg1FlQfcJlsSd2o1VmZAsydx/Vh3gxWvtHvqSyFV61wiqqXpKRpmZ6FKeY2q64RiOYs+TYzWpp+FKug+DLr9B6z0gF2YZM3fNpGxmkcq2yGMO1LZu8ZlJmoQjlumACEDccstchzw1tOQQrOZNoQMBE7B+qSLYBcFgg4pIPD3jDMQUMzCxCypSGt6zZYQN5tOXtHJzJRHxedyG9Q8L5OoS0SXvQ2cMGzIVOAWy8VM7PIAIGfx6oQ1A+ub6wR1HO6AfzSQmaXAkThHUF8Xv5c99rvKmfu3ye3EJzuID09MTHWkJj+SaZxYEFT06xBoc580893hSISZec7Ld4fPgJbp3eFNVWk6W4+hLZ0soMv3rvO963zvOt+7zveue3eZ8t3rfPc6WkPy/et8/zrfv873r1/F/et9VF/iRjDfu44++Sbg9MLeLKfo7vkXU50P27LaBiMf1IygZPKyA4BRgkz/iAATYjQ8W4bpA7TfmG/F57xJn63tDj5tIneL7GmT+ttbfM5EAnTnTOobWfAhEPZZjSgZZuAYB5NhG4C2DDMAMd9kTQapc4In+ozAlqIpZrrT2zneE30aIAP4zj5owUHaBxeijXumDlhkCS18gIH9gQ7pjnGbw1Xeohzwuge7M5WyVWY932YiSHl4UL0lhpUODNgLS3klBzUcLIwBPdHmYb08rJeH9fKw3isd1stPC0UizE8L5aeF8vM4+Xmc/DxOfh4nP48jwBmgV5IfyMkP5LR5EhiIa5q2D2qbvZTjcZtET9l3eWxpB5hmwYt6SlFzH5+YKS8AZViEFEJLRCUpv6cM2jFgGMmaF3vOvUJGZkvRs+BxPsVKvZHy9OaKXNZlfPJ10WY7qPoKaXO+WuWrVWft+FqtVruU1BQVB9/8zMO2edg2+2FbfgAsk8gyHVBm+Pb2W/ZKs4DsMdmpMXkZKYbp9hUN8+XmCKkpn9xgSDJwxDHffsi3H/Lth3z7Id9+6Nmdzg+HCRJJ9exPfkAtYBXzA2r5AbVX4IBaRcI6ogrJYxp5TCPw+FveeYDAK8vks3kecOkDGdiuEvuDqjIJMNMRoWx/IFkGokJ5ECQPguRBkDwIEqu7j45wiTQ7f5D04OdQqrGZSJcRG6wZ8zEs71lbmvawwlwiBanKlzhj0LaRRMkDXGOP2hVslvWmZRrrkqkcRX0mBfAWbeYi4y7a7EWXv0PHBv7RH0K/9iy9qx4xvux2Zb3GTNGZPeFc2e5ISNegxe41zebuYHP09cpT93m+GmoqRf3ropcwaP10j5VLTxs79cvXxd665dY98FV2i0jOF7CEOwS5RT871UNfzvoWhvi4GF74uNfkyXjxZzw4l2+SiNJINQBtb0+AuFM+cpDv1mRnt2aw+yIJ2xzcRBSZhBplvUYSNDj8u9dYa+kO3QaWFA2pA8UR3wDa/A2iePW0qQE6bukKa9LpN/+0yo+w/5Fsu5TJgZ6yJMe0+41wtCqWmFIUT5rIbKzNzM3Pa4apGyv2h3M637o5HyhTU7AquwVsbpgj8yJSG1M7kK5QGaileIDuJwOUuXCfbgFahupO74D4G5hng/LMzJmc3vuP/Ql7MQZhCwtUktK+fV6ooS+OTRJrHGL1PiQxbqBO3WDlwCwkAMh+EupTdnfPK7vwd2wljPe9uPRyABbrXj+QMmGzArNrIRaRJ2i3vNfuGTDhcat/Y+B+dmFiQEEY8YIdhHi5zsULO6FZ2PpBDD3Z3vCHOKQ9HfkmWiyCd7bj4pa38NpxLDDF15hjByu8VRoLWPEt1djBRr0iV41eEEtEZw9YiD0iP45/2Yx8VS/R3noWrdpmNerU3/MvWtGHqWPvceCcYBoDGzyomFj/Uh7N1ohvHD09xKcU16JGMqI9xolp5wFPri8t6xPvkI2/XYcCT3DtOxR8akyuC2KYuodeCEtJSNUd/C1rVzLzJnh8qt9haGOVzjEU/do54dWKHjoTtYx07lMXC2CyHe1n6gguQefetfgiyfYl5KT0Nn2iXYDzzaI+3Yq+J1PQuY9y9Z3+RD30DPL5obe+nN2NxHsQ/VzTtXKFnwjPp1Y9P1/GrVCtMz0GhRqg1erQkT5NVl+96N1eCfsmQiDHge5tzsQfCfK/TK3fpb0Vbj/LeS+Y/S9X6wMzV7Au/JBul+dBa3i82j0AzW4VfDBkfF7ZnzcA3au+d9eFbvW+ny6cc8mK1REapAfkbNW07NxEiH8xsV2gqC2uru07l1Lr5A3sa3dtLwe7rMa5oA5iKXX9msiZ2p/AB2Bpgm5AJPbenYHBmpfAwYpzu8ODNS2B0ysRZuVuIqdgzrQnobM+9nkhqYE1dP/i64VC4X8vrspKrVanK/Y/pBVPNJXVbAcf12YsqjsFjFuaIlFikJp5SyLaCuO7ZXPNOGXsKs4q4zZ064iZ2lVPRnYdZ5+Iur/qC73oYFdkcSj8wxGUHO/AyMLZqfur5Y37C6vz7LoK8db7jwiRV+f57eq8X/rs+pci6l+0618U6n+AoqsPLRxiG6Gs6I64BRrIKDX497+tzSi6gamJQTotfRPaXggimQ+11wu2aCF0g02QiwBm8SxowdOEIrJgTl9Cc08Q3p9dnffuV/0TfffnVucFanU+2CZL8PSY3Ydm1P3RMTbTvrNuNLG+j6XGHOedA+Y5r1iJ6CYlqorpZcZ8sUqOdUzfrAacJJ/nG3YGmGU/0edWgtzfrkYFnfz8m1U3tFsxLfk0lHu9KhhTP/kNJzmIwWVWwni9pzQRr5cYrOQtPyPU6Ijw82ZYoE8JPTwg5PACE+BspLTb9P9C2+GJAHd27Upr7cuRBTqPCpRbjCzXabSg1C9EloocRWD/+Q7srX3vVHlEz6PlGqEN7eXaRkugwK3OBSI6C38TQ3D5BlzegMt1uHwTLm/C5S24vA2Xd+ByAy434fItdhkdZ5cb4Wb5B21sIx3V7Vac+TtRNRoYm9uoeYa63gxnVqCcU2sziLsIKCbZpRgutC5J2DA2MTItCuWWGdPr/A02ZOKKolkqf/PmyrosByn4Ck/UbCp63aEcqztmU8Zl9t8dXuN1eHtDY2Ul+E7rJjO1+KptUx/qRwolOvgaV+yUPUuHgZi2Kb/R1+BVXHuICDTAabjZJzx1aoP5LCZ2RTT98KRJqOmXny5rwYRJOwGquFbmdj2wWzVlp7FsTl71SHdGOAwueY2hUGqngTresNN8WdkFvVSRdOu5uk2Ogptw1yAlVMdlJ80n3PKv7SLLEOQ2bb8C6ydc28NauIlpJ00spQVa9ROcgZ70Eowp79bugUd6mOwUTx+mPJpnX2FjLmhXpQGrcB3pypeYTgHlZ05VTNL0ybeeKPjYfuFS0CSY9Fchh83jmlK3KOcdh5QtwjQHbhw1A9bXgfbrhKRpSLJjSPYM5TwufnvSXBOTHCmN9P7zTnhKcmfCbgJmcJ6f5+f5eX6en+f3kw9/Q//z8uXLn7K/YSD+2yF4zn+JxH+KxI9F4j9E4t/F2v5NJP5VJP5FJP5ZJP5JJP5RrPofROJHIvFDkfh7kfg7kfhbkfgbkfhrkfgrkfhLkfiBSHxfJP5CJP5cJP5MJP5U7Nz3ROK7ItufiMQfi8QficQfisQfiMTvi8TvicTvisTviAh+WyS+EonfEonfFInfEGv7dTHn10TiV0XiV8QyvywSvyQQI5fY5avhyqlhYm2uBA9cEnhgxtwjzB6FFGluQ+EJiJ5+vvTsmcNY4S9IzhY1QyJUVQ5mi0+cbzS+PbcAv7PFkqXCA82aji2TInW2uGsdqIr0ET7dJ4dYXzu4exfdke68t/j+8m28cO/957PPekVR1s3lpYRA7By8YBjirfx5zNXBOI859YyXiNZEFNPxD5HRqDC/vTBcGP/FoQ4ydf4//MJ+mnAr+Hwx0WF+Do/ihYn9gv0zBoGzAjwiT4M6vhU2pWXXvQdtvTI9dsVlH4G/Fstb9h8ieIGR6SmnoenXnJsRaGjK6aHTH6jsYnUbvSCU/VN0+PfAUlR5orqHjxRggaLj7OeCU81L52cUIhI9B67GqiZ/DHNCDsMjNyIGCkaSs3UdhfRiDp/ABQKYoxAr6TpMNlTwoiAjvTfK27t+pjgi4k2T1SP3wTQpiTz1EELMqN/QXtLj9pmHEoJa/QUSk8b4zMMIMbcew5ZJg3vugYNYYPdB0hg0/50zpBHS+xhavNF2bkeEamNo72bbud0m2htDmxC+7T1gnLSaVT18xcJZgeAhbuAU+HRHaHG4IxReO4JlClbILK7ffA2F9aVjP0A2k1sEyZsIdsxb3JRp4Cyx0WM290iRBb9lhLVtXHyCVAsbhcLwcGF09NJ4VFtlt653ozJb6v/Jx/c+AOyTk+A3TRzARQJnAlYG6E+IQYYLBobPohlqcKkDw7NohgZcFGB4Hs3wAi6HwFCNZlDhogEDimYAt2SCsMv0geOXTEvujezeYPem5t7U3ZuGe6O4Ny/cm0P3RnVvNPdGd2+Ic3Pp/wEAAP//AwBQSwECLQAUAAAACACJXbdW0cBols4SAABf1gAAGABgAAAAAAAAAAAAAAAAAAAAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU4AE5VQ1gYAAAAQQBzAHAAZQBuAFQAZQBjAGgALgBBAFMAVwBYAEwALgBXAG8AcgBrAGIAbwBvAGsACgAgAAAAAAABABgAl64UYkqN2QGXrhRiSo3ZAeiPEGJKjdkBUEsFBgAAAAABAAEApgAAAEYTAAAeAEFTV1hMIFN0b3JhZ2UgVmVyc2lvbiAzOC4wLjAuMA==</t>
+    <t>AGES-GL-08-001_Process Design Criteria.pdf</t>
+  </si>
+  <si>
+    <t>AGES-GL-08-002_Vessel Sizing Guideline.pdf</t>
+  </si>
+  <si>
+    <t>AGES-GL-08-003_Flow Assurance Guideline.pdf</t>
+  </si>
+  <si>
+    <t>AGES-GL-08-005_P&amp;IDs and PFDs Development Guideline.pdf</t>
+  </si>
+  <si>
+    <t>Doc. Name</t>
+  </si>
+  <si>
+    <t>ASWXL Storage Version 40.0.0.10</t>
+  </si>
+  <si>
+    <t>C:\Program Files\AspenTech\Aspen Simulation Workbook V14.0</t>
+  </si>
+  <si>
+    <t>UEsDBBQAAAAIAA9yIlu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgAD3IiW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYAGO3mabyG9wBY7eZpvIb3AEK85im8hvcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
   </si>
 </sst>
 </file>
@@ -279,16 +210,6 @@
   <dxfs count="7">
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -309,11 +230,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FFFF0000"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -324,6 +245,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -648,108 +579,63 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.109375"/>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="98.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="58" customWidth="1"/>
-    <col min="13" max="13" width="14.5546875" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.6328125" customWidth="1"/>
+    <col min="4" max="4" width="53.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" s="3">
-        <v>45024</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -757,34 +643,14 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="3">
-        <v>45024</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -792,34 +658,14 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N4" s="3">
-        <v>45024</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -827,34 +673,14 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="3">
-        <v>45024</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -862,34 +688,14 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" t="s">
-        <v>41</v>
-      </c>
-      <c r="N6" s="3">
-        <v>45024</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -897,34 +703,14 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N7" s="3">
-        <v>45024</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -932,34 +718,14 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" t="s">
-        <v>43</v>
-      </c>
-      <c r="N8" s="3">
-        <v>45024</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -967,34 +733,14 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" t="s">
-        <v>44</v>
-      </c>
-      <c r="N9" s="3">
-        <v>45024</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1002,34 +748,14 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="H10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>34</v>
-      </c>
-      <c r="K10" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" t="s">
-        <v>45</v>
-      </c>
-      <c r="N10" s="3">
-        <v>45024</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1037,34 +763,14 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N11" s="3">
-        <v>45024</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1072,59 +778,39 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="H12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" t="s">
-        <v>47</v>
-      </c>
-      <c r="N12" s="3">
-        <v>45024</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G12" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N12" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G12" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="duplicateValues" dxfId="6" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1041371">
     <cfRule type="duplicateValues" dxfId="5" priority="240"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D11 D13:D1041371">
-    <cfRule type="expression" dxfId="4" priority="239">
-      <formula>AND(COUNTIF($D:$D,$D2)&gt;1,$F2="closed")</formula>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="duplicateValues" dxfId="4" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="expression" dxfId="3" priority="250">
+      <formula>AND(COUNTIF($D:$D,#REF!)&gt;1,#REF!="closed")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
+  <conditionalFormatting sqref="D1:D11 D13:D1041371">
+    <cfRule type="expression" dxfId="2" priority="251">
+      <formula>AND(COUNTIF($D:$D,$D2)&gt;1,#REF!="closed")</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1041372:D1048576">
-    <cfRule type="expression" dxfId="2" priority="21">
-      <formula>AND(COUNTIF($D:$D,$D1)&gt;1,$F1="closed")</formula>
+    <cfRule type="expression" dxfId="1" priority="253">
+      <formula>AND(COUNTIF($D:$D,$D1)&gt;1,#REF!="closed")</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="1" priority="22"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="0" priority="250">
-      <formula>AND(COUNTIF($D:$D,#REF!)&gt;1,#REF!="closed")</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" dxfId="0" priority="254"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1138,19 +824,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Update Master Index.xlsx to reflect recent changes
</commit_message>
<xml_diff>
--- a/check/Master Index.xlsx
+++ b/check/Master Index.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\sortx\check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4375FBCD-42D1-4396-A73F-902A04B8ACB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E032CE2-F7E1-47E4-9EDC-275E2898656F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ASWXL.Storage" sheetId="5" state="veryHidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,50 +37,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
-  <si>
-    <t>ELECTRICAL</t>
-  </si>
-  <si>
-    <t>S.No.</t>
-  </si>
-  <si>
-    <t>Discipline</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>OVERALL SINGLE LINE DIAGRAM 380V MSB</t>
-  </si>
-  <si>
-    <t>Overall Single Line Diagram (380 Main SB)</t>
-  </si>
-  <si>
-    <t>EB-1801 6,6 KV SWB METERING AND PROTECTION</t>
-  </si>
-  <si>
-    <t>H-0830 ELECTRICAL CABIN EQUIPMENT LAYOUT</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ABK0908-08-E-38-050_03-03</t>
   </si>
   <si>
-    <t>ELECTRICAL EQUIPMENT LAYOUT AND CABLE ROUTE - BOAT LANDING AND CELLAR DECK</t>
-  </si>
-  <si>
     <t>M-A26-EL-LYT-43-311</t>
   </si>
   <si>
-    <t>ELECTRICAL EQUIPMENT LAYOUT AND CABLE ROUTE - MEZZANINE DECK, UPPER DECK, HELIDECK</t>
-  </si>
-  <si>
     <t>M-A26-EL-LYT-43-312</t>
   </si>
   <si>
-    <t>ELECTRICAL EQUIPMENT LAYOUT AND CABLE ROUTE - MEZZANINE, UPPER AND HELI DECK</t>
-  </si>
-  <si>
     <t>M-A27-EL-LYT-43-411</t>
   </si>
   <si>
@@ -123,7 +90,7 @@
     <t>C:\Program Files\AspenTech\Aspen Simulation Workbook V14.0</t>
   </si>
   <si>
-    <t>UEsDBBQAAAAIAA9yIlu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgAD3IiW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYAGO3mabyG9wBY7eZpvIb3AEK85im8hvcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
+    <t>UEsDBBQAAAAIAItyIlu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgAi3IiW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYABChMzHzG9wBEKEzMfMb3AEmBTMx8xvcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
   </si>
 </sst>
 </file>
@@ -207,7 +174,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -215,16 +182,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -270,11 +227,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FFFF0000"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -579,236 +536,122 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.08984375"/>
-    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="98.6328125" customWidth="1"/>
-    <col min="4" max="4" width="53.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="79" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" customWidth="1"/>
-    <col min="7" max="7" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G12" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1041371">
-    <cfRule type="duplicateValues" dxfId="5" priority="240"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="3" priority="250">
-      <formula>AND(COUNTIF($D:$D,#REF!)&gt;1,#REF!="closed")</formula>
+  <autoFilter ref="A1:D12" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A1:A11 A13:A1041371">
+    <cfRule type="expression" dxfId="5" priority="251">
+      <formula>AND(COUNTIF($A:$A,$A2)&gt;1,#REF!="closed")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D11 D13:D1041371">
-    <cfRule type="expression" dxfId="2" priority="251">
-      <formula>AND(COUNTIF($D:$D,$D2)&gt;1,#REF!="closed")</formula>
+  <conditionalFormatting sqref="A1:A1041371">
+    <cfRule type="duplicateValues" dxfId="4" priority="240"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="expression" dxfId="2" priority="250">
+      <formula>AND(COUNTIF($A:$A,#REF!)&gt;1,#REF!="closed")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1041372:D1048576">
+  <conditionalFormatting sqref="A1041372:A1048576">
     <cfRule type="expression" dxfId="1" priority="253">
-      <formula>AND(COUNTIF($D:$D,$D1)&gt;1,#REF!="closed")</formula>
+      <formula>AND(COUNTIF($A:$A,$A1)&gt;1,#REF!="closed")</formula>
     </cfRule>
     <cfRule type="duplicateValues" dxfId="0" priority="254"/>
   </conditionalFormatting>
@@ -828,15 +671,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Update Master Index.xlsx to address discrepancies in data
</commit_message>
<xml_diff>
--- a/check/Master Index.xlsx
+++ b/check/Master Index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\sortx\check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF589E7-954A-406A-BB02-166EBADAE68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D87F6A-9C87-485D-A31E-98B22B1952DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UnMapped" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="1476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="1476">
   <si>
     <t>ABK0908-08-E-38-050_03-03</t>
   </si>
@@ -4465,14 +4465,14 @@
     <t>C:\Users\IDM280307\Desktop\2.01 ADNOC\AGES\Telecommunication\REF\Wireless Infrastructure and Communication System Specification.pdf</t>
   </si>
   <si>
-    <t>UEsDBBQAAAAIAKV0Ilu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgApXQiW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYAE1ILor1G9wBTUguivUb3AGiMySK9RvcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
+    <t>UEsDBBQAAAAIAEN1Ilu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgAQ3UiW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYADTrdzr2G9wBNOt3OvYb3AGf43A69hvcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4484,6 +4484,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4532,10 +4540,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4546,8 +4555,13 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
@@ -4913,9 +4927,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3FA8C0-63A1-4C88-8506-64C2ADF951E7}">
   <dimension ref="A1:C741"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="108.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="173.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -13078,25 +13099,26 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="53.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
+      <c r="B1" s="6" t="str">
+        <f>HYPERLINK("C:\Users\IDM280307\Desktop\2.01 ADNOC\AGES\Process\AGES-GL-08-001_Process Design Criteria.pdf", "Open File")</f>
+        <v>Open File</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
@@ -13109,8 +13131,9 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>354</v>
+      <c r="B2" s="7" t="str">
+        <f>HYPERLINK("C:\Users\IDM280307\Desktop\2.01 ADNOC\AGES\Process\AGES-GL-08-002_Vessel Sizing Guideline.pdf", "Open File")</f>
+        <v>Open File</v>
       </c>
       <c r="D2" s="3">
         <v>45902</v>
@@ -13120,8 +13143,9 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>356</v>
+      <c r="B3" s="7" t="str">
+        <f>HYPERLINK("C:\Users\IDM280307\Desktop\2.01 ADNOC\AGES\Process\AGES-GL-08-003_Flow Assurance Guideline.pdf", "Open File")</f>
+        <v>Open File</v>
       </c>
       <c r="D3" s="3">
         <v>45902</v>
@@ -13153,6 +13177,10 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
+      </c>
+      <c r="B7" s="7" t="str">
+        <f>HYPERLINK("C:\Users\IDM280307\Desktop\2.01 ADNOC\AGES\Process\AGES-GL-08-005_P&amp;IDs and PFDs Development Guideline.pdf", "Open File")</f>
+        <v>Open File</v>
       </c>
       <c r="D7" s="3"/>
     </row>

</xml_diff>

<commit_message>
fix: Remove unused __add_hyperlinks method from FileCrawler class
</commit_message>
<xml_diff>
--- a/check/Master Index.xlsx
+++ b/check/Master Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\sortx\check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D87F6A-9C87-485D-A31E-98B22B1952DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE7C406-E45B-40D7-AF09-85C89CC2ACDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="1476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="1477">
   <si>
     <t>ABK0908-08-E-38-050_03-03</t>
   </si>
@@ -4465,7 +4465,10 @@
     <t>C:\Users\IDM280307\Desktop\2.01 ADNOC\AGES\Telecommunication\REF\Wireless Infrastructure and Communication System Specification.pdf</t>
   </si>
   <si>
-    <t>UEsDBBQAAAAIAEN1Ilu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgAQ3UiW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYADTrdzr2G9wBNOt3OvYb3AGf43A69hvcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
+    <t>Open File</t>
+  </si>
+  <si>
+    <t>UEsDBBQAAAAIAEB2Ilu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgAQHYiW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYAPnhplT3G9wB+eGmVPcb3AHOjp9U9xvcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
   </si>
 </sst>
 </file>
@@ -13116,9 +13119,8 @@
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="str">
-        <f>HYPERLINK("C:\Users\IDM280307\Desktop\2.01 ADNOC\AGES\Process\AGES-GL-08-001_Process Design Criteria.pdf", "Open File")</f>
-        <v>Open File</v>
+      <c r="B1" s="6" t="s">
+        <v>1475</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
@@ -13131,9 +13133,8 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="7" t="str">
-        <f>HYPERLINK("C:\Users\IDM280307\Desktop\2.01 ADNOC\AGES\Process\AGES-GL-08-002_Vessel Sizing Guideline.pdf", "Open File")</f>
-        <v>Open File</v>
+      <c r="B2" s="7" t="s">
+        <v>1475</v>
       </c>
       <c r="D2" s="3">
         <v>45902</v>
@@ -13143,9 +13144,8 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7" t="str">
-        <f>HYPERLINK("C:\Users\IDM280307\Desktop\2.01 ADNOC\AGES\Process\AGES-GL-08-003_Flow Assurance Guideline.pdf", "Open File")</f>
-        <v>Open File</v>
+      <c r="B3" s="7" t="s">
+        <v>1475</v>
       </c>
       <c r="D3" s="3">
         <v>45902</v>
@@ -13178,9 +13178,8 @@
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="7" t="str">
-        <f>HYPERLINK("C:\Users\IDM280307\Desktop\2.01 ADNOC\AGES\Process\AGES-GL-08-005_P&amp;IDs and PFDs Development Guideline.pdf", "Open File")</f>
-        <v>Open File</v>
+      <c r="B7" s="7" t="s">
+        <v>1475</v>
       </c>
       <c r="D7" s="3"/>
     </row>
@@ -13266,7 +13265,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Update Master Index.xlsx to reflect changes in data structure
</commit_message>
<xml_diff>
--- a/check/Master Index.xlsx
+++ b/check/Master Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\sortx\check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE7C406-E45B-40D7-AF09-85C89CC2ACDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EDF9B0-7E29-4F64-8831-5755282D8E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4468,7 +4468,7 @@
     <t>Open File</t>
   </si>
   <si>
-    <t>UEsDBBQAAAAIAEB2Ilu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgAQHYiW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYAPnhplT3G9wB+eGmVPcb3AHOjp9U9xvcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
+    <t>UEsDBBQAAAAIAF12Ilu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgAXXYiW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYAPKTD3f3G9wB8pMPd/cb3AFd3gh39xvcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
fix: Clear File Path column before writing to Excel in FileCrawler class
</commit_message>
<xml_diff>
--- a/check/Master Index.xlsx
+++ b/check/Master Index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\sortx\check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EDF9B0-7E29-4F64-8831-5755282D8E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A06BE0-D902-4F81-BA59-A4A97E288B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UnMapped" sheetId="6" r:id="rId1"/>
@@ -4468,7 +4468,7 @@
     <t>Open File</t>
   </si>
   <si>
-    <t>UEsDBBQAAAAIAF12Ilu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgAXXYiW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYAPKTD3f3G9wB8pMPd/cb3AFd3gh39xvcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
+    <t>UEsDBBQAAAAIAKB4Ilu9mOgA3hIAAP/WAAAYAEIAQXNwZW5UZWNoLkFTV1hMLldvcmtib29rTlU2AE5VQ1gYAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoABAAAAAAA7F3pc9s4lpdjO7GdxO10pjN9JDMqV2/V7JbjK0knnbLT5chxWtV2nLbcSc+mUmqYhCTEJKEGSR/9T2zV/h977/bu7Dmzxxx73/fsftiv830+ZvHAC6QoWZJFkdOhXaYJ4AH4vYeHh8cHUCqMFAqFl/wH/sPPhTP88otrZhMbu1hpzK9Vnn66Ob+mqsSYKz7BzCTUWL25OA+/S4tzxZKtWTbDqwa2LYa0ueJje08jykf4eJfuY2N1ESnKrRvK4p33a8uLd9TaOHT0ZrT9p5Tt71G6f5kXjlYPlAtVk+i2hizem3mpihSLHOCKn3Wh2mS4hhk2FGxeqBKDWARp5AusTld1ZFqYrSMLVbB1JZycdxl4Q8ouUcNiVNMwu1hlyKjjLWSgOmYXqnVG7eaawrswL1eRbVGdd67sovonTRVZ+Fp1HWvYwrtoT8NPG9gQSWLUd6CVn6vagurBkYK1DdtQBCtAts1Z9/h9u2qiA7xJjH2scva2eRuCV17xqih6oO9hVW0p/Ga1RpmCN2xN28E1hs3GtrFjGyWqNwGSCiID3BsYwehsoeaVqgU472vI2C9RDbjGhmW+XUXmoeBgTSB8jAz8wIC0OjZ2ZqzAf8fGHM0YGy3MRsftCWIEiEsgQNEAqM+tKFlQbDo5wVCGa74brfnYH+cw4cg3opQwls4t3AHNxLc60wQjD9RXo8Q7kjIAwTtRgoeBfghI4qfYMnUiAwGkX45Wjrn+6SHBPMQGZkSZXyciA7Hjz5afPXMJKxbjmjVX1E2FMo3sSXNRTMUuZuLe7dvolnLrvaX3b9zEfD4+n3vWK4qyYd1YTgjE9t4LjmGwjT8fcHMjMHiTo3CBSTE1OQ7jPnkWrpB5Di4T/DL+U25SOykMkJ87QJqNq9XCBDQLrXId4g1NTkEz5yE5DrldzrqzVcQYOj5bVahtWGOt+lr26j17LqaHYOaCa/fHx041caOdX2vpPKgpd3/R636829kPMp7apEjd4MaQsnPusE6A7UMMs5kPkdkoURU/ZvSAqJhNQEaFLw5jfGTNs09A6CaX9yjv9PzE1Zg5UPbaejeusKV9YOQnH9/5APiYmhLaMQ2X14Av0I0TbBXU+Lq3Qu1gncIi4rI1+amuVZQG1tF5frdOarWHDOmjIyPTLjSXTghzBgbiEr/80o/PrHxwpGvFA1fnZ5fmF2eLXJCUr+P11Vnbql1fem/2g3sXp1aOzLum6KFI1NVZH9Vs0UKsjq1HSMdmEyl4dbZhWc27Cwu826bNyDxl9QWgNLG1NH9kqrNF3qVh3tVNyzC7pe661aOA9PDwcP7whqBcXlxcWvh0a9ORUYCAL72Is8kMlzfzuk4URk1as64rVL/L6a47VEGdJqPNk+sA1WwRWdwg79kW3qBMX8c1xG3J6uznNvdCagRz0NwX0PkC26aYy71YBMm7ZEWDSzkkfAfc3bLpKsbqrMVs7Od/YuKSzfjUsDapgjTsFot2nZYV4Qsc7R43sZvr5jcoUXBRJ8a2otiMS5Vrho6OvJRt7PEprHogg4phqNwN8swJgAKp3JW0bVmu3R5QUGriz22Y6JGiuK7L674YdjBStw3tOCKdNe6slQ2FiVpemcU7Xp3lrRHD8il71/GFLhBCe1KHpli8E+5zHZsKI00wUoPsOqwn3QARBlaCoFLbVZKhQfiEPxCY6UrhY5jr1nG6IITDkS4E4UUPcSxWFtoZE1ESb4REkYu7C6u3287qLb7SVi8zFkjoXLoQuJP4IR8lzHbooYSEP/NrGHHxqJ5PUEOaOVzjyKFJI5U9fKDG4DYhK90hvE8ZH781Bt7QwOZRf+J4SlSrkbFhEkawYh1rKc+0XWJlAgdMd95nBpCUDQMzR3tT1NstzPtYM9QSzwoB8ZV3iGAqFrLsOC/En0DbH/3suySbxLQS9EBEH+CGDNGnKDWIpg65T74kbtdqvM6QZk/i+rHmBSteafc0kEKq1rlENVs3UjTM7kKV8hpVNyjDahZ9mgFam34WqrD7MOz+7/PaQ3ZhkjV/W1TFWh6pbIdw0JHK3jUuM1GDaNwyBQgZiFtu0sOQt56GFJrNtCFkIHAK1iddBI9RKOiQAoJgzzgDAcUsTMyShvSm320JCbPplhXdwkx5VGIut0EtyjKJukQN1d/AicKGQgK3WC1mYpcHALmLVyesGVjfPCeo43CH/KOhzCwCR+JcQX1V/F7+2O8pZ+7fJrcTn+wgPjiyMDOQlvxIpnFiQVLRr0KgzXvSzHeHYxFm5jkv3x0+AVqmd4c3NNJ0tx4jWzpZQJfvXed71/nedb53ne9d9+4y5bvX+e51vIbk+9f5/nW+f53vX7+K+9e7qL4sjGC+dx1/8k3C6Ye9eUnR2/MvpjoftlStDUYxqBlByeXlBADjBJn+EQEuxHh4jgzTB+i8Md+Kz32TPlvbHWLaxO4WOdMm9be3xJyJBejNmdQ3suBDIJyzGnEyzMAxDi7DNgAdGWYAYr7JmgxS9wRP/BmBTaITK93p7R7viT8NkAF8Jx+0ECCdgwvxxj1TByyyhBY+wMD5QId0x7jN4Sp/UQ553cPdmUrZKnPOt7gIUh4eVG+JYaUDA/bCUl7JQQ2HC2NIT7R5WC8P6+VhvTys90qH9fLTQrEI89NC+Wmh/DxOfh4nP4+Tn8fJz+NIcIboleQHcvIDOW2eBIbimqbtgzpmL+V43AY1UvZdHtn6HmZZ8KKeMtTcxUdWygtAGRYhQlmJajTl95RBO4YMI1nz4sy5V8jIbBIjCx7nU0zqjZSnt1DksqHio6+KNjtB1VdIm/PVKl+tOmvHV2q1esxojWg4/OZnHrbNw7bZD9uKA2CZRJbpgDLHt7PbsleaBWSP6HaNy8tMMUy3S3QslpsDpKV8coMjycARx3z7Id9+yLcf8u2HfPuhZ3c6PxwmSSTVsz/5AbWQVcwPqOUH1F6BA2oVBRuIEZrHNPKYRujxt7x9H4FXlsln8zzg0gcysF0l/gdNZRJgpiNC2f5AsgxEhfIgSB4EyYMgeRBkoO4+OsAl2uz8QdLDn0OpxmZiXUZs8m6sR7C8Z21p2sGEu0QEaeQLnDFoW0hh9D6u8UftCrbKRtO2zDXFIgdxn0kBtEWHuMipiw550aPvwNjQP/pD4mvHNrriiNNll5W1GjdFJ3IiqLLNSETXoMfuNc2h7mBzjLXKU+95vhrpKkX964JLGLR+2OP10tPGTnwFutgbW17bQ19lN6nifgFLlCEoLQbFqR76cte3KMRHxejCJ7wmX8ZLP+PBuXyTRJZGqgFoZ3sCxJ3ykYN8tyY7uzXD3RdJ2ObgJmLIoswsGzWaoMER373Ge0t36NaxQnSkDRXH4AbQoW9Q4rfTpgVg3DYI79LlW3xa5Uc4+Ei2x4zLgR3zLNe0B50ItBpWuFIUj5rIaqzOzi8s6KZlmHedD+d0v3VzIVSnRrCmehUcapgjCzJSB1M7kFLjIP0SNfjIIJhbSYBzPLUe4HljzmW2PBg57iYjR+5hfroJaDmqW70DEi+IngzKt4InUvqvZ/Yn7KUBCFtaP5OU9s3TQo18r22SWAchVv8zHBMwBdA2zFGwWgkA6nn6y7K7fVrZRb8CLGG87w1KL4dgse70AykTNis0uxYHIvIE7Zb/qQAcmPQ02L8x8D5aMTGgIIzBgh2GeIXODRZ2QrOw9XMierK90c+YSHs6ij2+gQje3S0ctLylt6IHAlN+y3rgYKWXXgcCVn6JduBg497gq8YviMFTxqPBL5uxbxImyq1v0aptVqNO/J5+0Yo/6z1wjkPHGNMY2PA5ysT4S3k0WwPSg+B0Hx8zXIsbyZj+OCVmnQc8OV5a1ifBkIO/HUOhJ7j2DIWfGpNjQY6i98CFtJREVN3F37J2JTNvwqe7+h2GNlbpFEPRr52T3vzogZm4ZaQzT10sgMky2s/UkVyCzty1+CLJ8hJxUnqbPvEuwOlmUZ9uRd+TKezcx7n6Lj9xDz3DfH7ojZeT2Uicg/jnmq6VK/pEeDq16vn5ctAK1TrTB6BQQ7RaHRjp02T1xUXv9kraOZECOS50f+9o8JGg4Lve+l3aW+H2s5z3gjn47rc+MAsF68IP6XZ5HraGD1a7h6DZrYIPh4xPK/vTBqB71ffuWOhW7/th4ZRL1kAdoWF6QO5WTcvOTYz4lxLbBYrb4uravgsptU7e0L521/ZyuMvqIBfUYSylnl8TO1P7E/gQLE3YDYjF3rszMFzzEjpYcWp3eLimJXR+Jcas3E7kHMyJ9iRyFMk5zqQ0sI7unX29UCj839kVldRqdXbX+Yf04pGu8Zad4OPqrM0Mt4J5XScKoyatWdcVqt/ldNcdqlm3jtPESXW8jq4fcFO74svIaePkA1v3VgKhF13sRJWHIjgcwejhNowsHO26t1Jev7e4ssCvKxBvvfeQUnVlQdyuLAS1T25/Oab9Jaf9Jan9+yi++cjCIfcRKYpnxKvQQGapIb6ebnWWGCZmFgbptPAm9b0YRrIQ6a8XbPFC6AabJBcJzNJJ0MKHHWVk4ZK+hOYdcLw3t7Lg368EBw7vza8sSKmVhXCfPMPXY34fmVH3xs/xmfatNbOJjV2sNOYF7TwQz/vVStSwGNU0zC5w4rNVemhg9mY15CQFNF9zCsAsB5kBNQlTf7MaF3QKyq9VvdBuxbLV40jplapkTIPsN9zsMAaPmETx+k9pMl4/M9zIW0FBpNMx6efNqECfUra/R+n+GS7AuVhpt+H/TNvhiQF3cuuktfUbsRU6jwrUW4qt12m0oNYvxNaKHUUg//kO5K28d2o8hvN4ucZoQ3u5ttESqHC9c4UYZuFvcgQuX4PLG3C5Apevw+VNuLwFl7fh8g5crsLlGly+wS/jE/xyNdqt+ByQLWSgutOLO38nq2YDY2sLNU9Q12vRwgrUc1tthnEXAcUUvxSjldYUBZvmBkaWzaDeDU70unjBDlm4QnRbEy8GXVxT1XAKvmEUNZvEqLsp1+qec1LmBf7fG17zdXi5ROd1FfjK7SY3tfiSY1MfGAeEUQN8jYtOzo5twEDMOKmg09fgTWFniCh0INJws0tF7vQ691ks7Ilo5sFRkzIrqD9T1sMZU04GNHG5LOx6aLdq2snjxSJ5yU96M8Il8JKXOQpSOw618YaTF8jKqejnykmvnUtb9CC8CXcZciJtXHDzgoRX/7XHyDYluc04b+gGGZd3sB7tYsbNk2vpoV6DDHegp/wMc9q/dTjwkz4mJ8fXh2k/LYov8jGXtKvSgFW4jgzyBWbTkAoKpysWbQbJt54QfOi8DyppEkz6S1DC53GN1G0maCcgZ5NyzYEbV82A9HVIB21C1gxkOTEkZ4YKGg+/M2kuy1mulMZ6/3knOiWFM+F0ATM4L8/L8/K8PC/Py/sph7+R/3358uVP+d8oJP7HTYiSH8uJ/5YT/yUn/lNO/Ifc2r/LiX+TE/8qJ/5FTvyznPgnuel/lBP/ICf+Xk78nZz4WznxN3Lir+XEX8mJv5QTP5ITP5QTP5AT35cTfyEn/lxO/JnM3J/Kie/JZN+VE38iJ/5YTvyRnPhDOfEHcuL35cR35MTvyQh+V058KSd+R078tpz4Lbm135RLfkNO/Lqc+DW5zq/KiV+REmPn+eXL0cqxaWF9vgQPXAp4YOb8Q8wfhYgyv05EBmLHny0/e+YSVsT7m3NF3VQo08jeXPGJ+4XLN+cX4XeuWLI1eKBZNbBtMaTNFR/bexpRPsLHu3QfG6t7t2+jW8qt95bev3ETL955//ncs15RlA3rxnJCILb3XnAMg238+YCbg3E+57YzUaJ6EzHMJj5EZqPC/fbCaGHil0c6yNT9/+Bz52nCa+CzpUSH+Tk8ihcmdwvOzzkInBXgEXkG1PGtqCkte+49aOvFmXMXPfIx+GuxvOXgIUJUGJuZdjuaec29GYOOpl0OXX6gsbPVLfSCMv6PGPDvvk00dbK6gw8IkEDVCf5zxm3mpfszDhGJngNX56qWeAxzQw6jY1djBgpGUpB1HYX0Yw6fwAUCmOMQK+k6TDZS8KMgY713Kvq7cqI4YuJNU9UD78E0KYk89RFCzKjf0F7S4/ZtHyUEtfoLJCaN8ZmPEWJuPYYtkwb33AcHscDug6QD0Px3TpBGRO8H0OPVtnM7JlQ7gP6utZ3bbaK9A+gTwre9B4yTVrOqj69YOCkQPCIMHIEPn4QeRztCEa0jWKZghczi+i3WUFhfOvIBspnapEjdQLBj3uKmzABliY8et7kHRJX8ljHet3n2CdJsbBYKo6OF8fHzE3F9lb223o0rbGn/Jx/f+QCwT02B3zS5BxcFnAlYGYCfCIEKFwwE344nqMGlDgTP4gkacCFA8Dye4AVc9oGgGk+gwUUHAhRPAG7JJOWXmT3XL5lRvBvVu8HeTc27qXs3De+GeDcvvJt970bzbnTvxvBuqHtz/v8BAAD//wMAUEsBAi0AFAAAAAgAoHgiW72Y6ADeEgAA/9YAABgAYAAAAAAAAAAAAAAAAAAAAEFzcGVuVGVjaC5BU1dYTC5Xb3JrYm9va05VOABOVUNYGAAAAEEAcwBwAGUAbgBUAGUAYwBoAC4AQQBTAFcAWABMAC4AVwBvAHIAawBiAG8AbwBrAAoAIAAAAAAAAQAYAGQd5235G9wBZB3nbfkb3AEd7t9t+RvcAVBLBQYAAAAAAQABAKYAAABWEwAAHwBBU1dYTCBTdG9yYWdlIFZlcnNpb24gNDAuMC4wLjEw</t>
   </si>
 </sst>
 </file>
@@ -13104,7 +13104,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>